<commit_message>
feat(xlsx): resolve threaded comment authors via persons parts
- Parse xl/persons/*.xml to map personId -> displayName\n- Use mapping when parsing threadedComments so authors are human-readable\n- Update comments fixture + test assertions
</commit_message>
<xml_diff>
--- a/crates/formula-xlsx/tests/fixtures/comments.xlsx
+++ b/crates/formula-xlsx/tests/fixtures/comments.xlsx
@@ -34,16 +34,23 @@
 </commentsExt>
 </file>
 
+<file path=xl/persons/persons1.xml><?xml version="1.0" encoding="utf-8"?>
+<persons xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/person">
+  <person id="p1" displayName="Alex"/>
+  <person id="p2" displayName="Sam"/>
+</persons>
+</file>
+
 <file path=xl/threadedComments/threadedComments1.xml><?xml version="1.0" encoding="utf-8"?>
 <threadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments">
-  <threadedComment id="tc1" ref="B2" personId="p1" author="Alex" dT="2020-01-01T00:00:00.000Z" done="1">
+  <threadedComment id="tc1" ref="B2" personId="p1" dT="2020-01-01T00:00:00.000Z" done="1">
     <text>
       <r>
         <t>Thread root</t>
       </r>
     </text>
   </threadedComment>
-  <threadedComment id="tc2" parentId="tc1" ref="B2" personId="p2" author="Sam" dT="2020-01-01T01:00:00.000Z">
+  <threadedComment id="tc2" parentId="tc1" ref="B2" personId="p2" dT="2020-01-01T01:00:00.000Z">
     <text>
       <r>
         <t>First reply</t>

</xml_diff>